<commit_message>
Versión 1.0.5 en PRD - Actualización versión en GIT
</commit_message>
<xml_diff>
--- a/Data/MD LC Direcciones ES&PT.xlsx
+++ b/Data/MD LC Direcciones ES&PT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/Stihl_LCE4_RT1_02_LimitesDeCredito/Data/TEST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/Stihl_LCE4_RT1_02_LimitesDeCredito/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{58FADFA7-C11E-491C-B5C9-58D93D7D7FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A92E37AC-B3DD-44E9-A4E0-1DDF453BB0CB}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{58FADFA7-C11E-491C-B5C9-58D93D7D7FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0729938-2E5A-4D14-A510-68B0DD33ACA5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51AEF158-A007-4ABD-BE96-B3908B24FFCF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Jefe de Zona</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>juvenal.martins@stihl.pt</t>
-  </si>
-  <si>
-    <t>icorral@rpatechnologies.es</t>
   </si>
 </sst>
 </file>
@@ -245,10 +242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -265,6 +261,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA84C72-B1C1-4FF3-97D4-9304E0A53EFC}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -597,7 +597,7 @@
     <col min="3" max="3" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -608,130 +608,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>47</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>47</v>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>47</v>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
+      <c r="B8" t="s">
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
+      <c r="B9" t="s">
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="I10" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +720,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="J4" sqref="J1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -949,6 +922,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -1183,27 +1176,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{297942C9-83ED-4EC2-B952-9B7446D4F4E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0380E2AF-2265-4CD4-B3A8-677DB6A6C380}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC2965B7-F2F6-46F7-B417-E5A5912FC764}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1220,23 +1212,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0380E2AF-2265-4CD4-B3A8-677DB6A6C380}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{297942C9-83ED-4EC2-B952-9B7446D4F4E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>